<commit_message>
[Alex Becker] - Priorização dos requisitos do 1 ao 3 e refatoração das decisões técnicas (java desktop e netbeans).
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso e Incrementos.xlsx
+++ b/Priorização de Casos de Uso e Incrementos.xlsx
@@ -468,9 +468,6 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -488,6 +485,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -796,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,57 +810,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="G1" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="1"/>
+      <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>4</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="G3" s="6">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="G3" s="5">
         <v>1</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>106</v>
       </c>
     </row>
@@ -871,15 +871,15 @@
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>4</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="G4" s="6">
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="G4" s="5">
         <v>2</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>106</v>
       </c>
     </row>
@@ -890,15 +890,15 @@
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>4</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="G5" s="6">
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="G5" s="5">
         <v>3</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>106</v>
       </c>
     </row>
@@ -909,13 +909,15 @@
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="G6" s="6">
+      <c r="C6" s="5">
         <v>4</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="G6" s="5">
+        <v>4</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>106</v>
       </c>
     </row>
@@ -923,14 +925,14 @@
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>4</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -939,11 +941,11 @@
       <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>4</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -952,9 +954,11 @@
       <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+      <c r="C9" s="5">
+        <v>4</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -963,9 +967,11 @@
       <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
+      <c r="C10" s="5">
+        <v>4</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -974,9 +980,11 @@
       <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+      <c r="C11" s="5">
+        <v>4</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -985,13 +993,15 @@
       <c r="B12" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="G12" s="1" t="s">
+      <c r="C12" s="5">
+        <v>4</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="G12" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="H12" s="1"/>
+      <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1000,30 +1010,32 @@
       <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="G13" s="7" t="s">
+      <c r="C13" s="5">
+        <v>4</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="G13" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="6" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="4">
         <v>4</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="G14" s="6" t="s">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="G14" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="5">
         <v>4</v>
       </c>
     </row>
@@ -1034,13 +1046,13 @@
       <c r="B15" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="G15" s="6" t="s">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="G15" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="5">
         <v>3</v>
       </c>
     </row>
@@ -1051,13 +1063,13 @@
       <c r="B16" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="G16" s="6" t="s">
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="G16" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="5">
         <v>2</v>
       </c>
     </row>
@@ -1068,13 +1080,13 @@
       <c r="B17" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="G17" s="6" t="s">
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="G17" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="5">
         <v>1</v>
       </c>
     </row>
@@ -1085,9 +1097,9 @@
       <c r="B18" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1096,13 +1108,13 @@
       <c r="B19" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="G19" s="1" t="s">
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="G19" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="H19" s="1"/>
+      <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -1111,13 +1123,13 @@
       <c r="B20" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="G20" s="8" t="s">
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="G20" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="H20" s="7" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1128,13 +1140,13 @@
       <c r="B21" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="G21" s="6" t="s">
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="G21" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="5">
         <v>1</v>
       </c>
     </row>
@@ -1145,13 +1157,13 @@
       <c r="B22" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="G22" s="6" t="s">
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="G22" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H22" s="5">
         <v>2</v>
       </c>
     </row>
@@ -1162,26 +1174,26 @@
       <c r="B23" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="G23" s="6" t="s">
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="G23" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H23" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+      <c r="A24" s="4">
         <v>5</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1190,9 +1202,9 @@
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1201,9 +1213,9 @@
       <c r="B26" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1212,20 +1224,20 @@
       <c r="B27" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+      <c r="A28" s="4">
         <v>6</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -1234,9 +1246,9 @@
       <c r="B29" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -1245,9 +1257,9 @@
       <c r="B30" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -1256,9 +1268,9 @@
       <c r="B31" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -1267,9 +1279,9 @@
       <c r="B32" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -1278,9 +1290,9 @@
       <c r="B33" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -1289,9 +1301,9 @@
       <c r="B34" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -1300,9 +1312,9 @@
       <c r="B35" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -1311,9 +1323,9 @@
       <c r="B36" t="s">
         <v>67</v>
       </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -1322,9 +1334,9 @@
       <c r="B37" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -1333,9 +1345,9 @@
       <c r="B38" t="s">
         <v>69</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1344,9 +1356,9 @@
       <c r="B39" t="s">
         <v>70</v>
       </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -1355,9 +1367,9 @@
       <c r="B40" t="s">
         <v>71</v>
       </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -1366,9 +1378,9 @@
       <c r="B41" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -1377,9 +1389,9 @@
       <c r="B42" t="s">
         <v>73</v>
       </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -1388,20 +1400,20 @@
       <c r="B43" t="s">
         <v>74</v>
       </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="5">
+      <c r="A44" s="4">
         <v>7</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -1410,9 +1422,9 @@
       <c r="B45" t="s">
         <v>79</v>
       </c>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -1421,9 +1433,9 @@
       <c r="B46" t="s">
         <v>80</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -1432,9 +1444,9 @@
       <c r="B47" t="s">
         <v>81</v>
       </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -1443,9 +1455,9 @@
       <c r="B48" t="s">
         <v>82</v>
       </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
@@ -1454,9 +1466,9 @@
       <c r="B49" t="s">
         <v>83</v>
       </c>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
@@ -1465,9 +1477,9 @@
       <c r="B50" t="s">
         <v>84</v>
       </c>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -1476,20 +1488,20 @@
       <c r="B51" t="s">
         <v>85</v>
       </c>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="5">
+      <c r="A52" s="4">
         <v>8</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
@@ -1498,9 +1510,9 @@
       <c r="B53" t="s">
         <v>94</v>
       </c>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
@@ -1509,9 +1521,9 @@
       <c r="B54" t="s">
         <v>95</v>
       </c>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
@@ -1520,9 +1532,9 @@
       <c r="B55" t="s">
         <v>96</v>
       </c>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
@@ -1531,9 +1543,9 @@
       <c r="B56" t="s">
         <v>97</v>
       </c>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
[Douglas Giordano] - Atualização responsábilidades no documento de priorização de casos de uso e incrementos.
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso e Incrementos.xlsx
+++ b/Priorização de Casos de Uso e Incrementos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="129">
   <si>
     <t>ID</t>
   </si>
@@ -365,6 +365,42 @@
   </si>
   <si>
     <t>Em Implementação</t>
+  </si>
+  <si>
+    <t>Responsável</t>
+  </si>
+  <si>
+    <t>Configuração do Ambiente</t>
+  </si>
+  <si>
+    <t>Configurações Gerais</t>
+  </si>
+  <si>
+    <t>Douglas</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Edson</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>Miguel</t>
+  </si>
+  <si>
+    <t>Vinicius</t>
+  </si>
+  <si>
+    <t>Gean</t>
+  </si>
+  <si>
+    <t>Gustavo</t>
+  </si>
+  <si>
+    <t>Finalizada</t>
   </si>
 </sst>
 </file>
@@ -560,7 +596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -580,9 +616,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -612,6 +645,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -621,21 +669,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -940,10 +977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,723 +988,794 @@
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="73.140625" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" customWidth="1"/>
-    <col min="8" max="8" width="28.85546875" customWidth="1"/>
+    <col min="4" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" customWidth="1"/>
+    <col min="9" max="9" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="G1" s="9" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="H1" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="9"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="I1" s="28"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="24" t="s">
+      <c r="B2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="I2" s="12" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="25">
-        <v>1</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="19">
-        <v>4</v>
-      </c>
-      <c r="D3" s="19">
-        <v>1</v>
-      </c>
-      <c r="E3" s="20"/>
-      <c r="G3" s="12">
-        <v>1</v>
-      </c>
-      <c r="H3" s="14">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="18">
+        <v>4</v>
+      </c>
+      <c r="D3" s="18">
+        <v>1</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H3" s="11">
+        <v>1</v>
+      </c>
+      <c r="I3" s="13">
         <v>42019</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="26">
-        <v>2</v>
-      </c>
-      <c r="B4" s="15" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="18">
+        <v>4</v>
+      </c>
+      <c r="D4" s="18">
+        <v>1</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="F4" s="29"/>
+      <c r="H4" s="11">
+        <v>2</v>
+      </c>
+      <c r="I4" s="13">
+        <v>42026</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="21">
+        <v>1</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="18">
+        <v>4</v>
+      </c>
+      <c r="D5" s="18">
+        <v>1</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F5" s="29"/>
+      <c r="H5" s="11">
         <v>3</v>
       </c>
-      <c r="C4" s="16">
-        <v>4</v>
-      </c>
-      <c r="D4" s="16">
-        <v>1</v>
-      </c>
-      <c r="E4" s="17"/>
-      <c r="G4" s="12">
-        <v>2</v>
-      </c>
-      <c r="H4" s="14">
-        <v>42026</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="27">
+      <c r="I5" s="13">
+        <v>42033</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="22">
+        <v>2</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="4">
-        <v>4</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="G5" s="12">
+      <c r="C6" s="15">
+        <v>4</v>
+      </c>
+      <c r="D6" s="15">
+        <v>1</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="F6" s="16"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="H5" s="14">
-        <v>42033</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="B7" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="26">
+        <v>4</v>
+      </c>
+      <c r="D7" s="26">
+        <v>1</v>
+      </c>
+      <c r="E7" s="26"/>
+      <c r="F7" s="27"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4">
-        <v>4</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="C8" s="4">
+        <v>4</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="4">
-        <v>4</v>
-      </c>
-      <c r="D7" s="4">
-        <v>1</v>
-      </c>
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="C9" s="4">
+        <v>4</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="4">
-        <v>4</v>
-      </c>
-      <c r="D8" s="4">
-        <v>1</v>
-      </c>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="C10" s="4">
+        <v>4</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="4">
-        <v>4</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1</v>
-      </c>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="C11" s="4">
+        <v>4</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="4">
-        <v>4</v>
-      </c>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="C12" s="4">
+        <v>4</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="4">
-        <v>4</v>
-      </c>
-      <c r="D11" s="4">
-        <v>1</v>
-      </c>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="C13" s="4">
+        <v>4</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="4">
-        <v>4</v>
-      </c>
-      <c r="D12" s="4">
-        <v>1</v>
-      </c>
-      <c r="E12" s="7"/>
-      <c r="G12" s="9" t="s">
+      <c r="C14" s="4">
+        <v>4</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="H14" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="H12" s="9"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+      <c r="I14" s="28"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="4">
-        <v>4</v>
-      </c>
-      <c r="D13" s="4">
-        <v>1</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="G13" s="13" t="s">
+      <c r="C15" s="4">
+        <v>4</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="H15" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="I15" s="12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
-        <v>4</v>
-      </c>
-      <c r="B14" s="21" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>4</v>
+      </c>
+      <c r="B16" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="23"/>
-      <c r="G14" s="12" t="s">
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="27"/>
+      <c r="H16" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="H14" s="12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+      <c r="I16" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="4">
-        <v>4</v>
-      </c>
-      <c r="D15" s="4">
-        <v>1</v>
-      </c>
-      <c r="E15" s="7"/>
-      <c r="G15" s="12" t="s">
+      <c r="C17" s="4">
+        <v>4</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="7"/>
+      <c r="H17" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="H15" s="12">
+      <c r="I17" s="11">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="4">
-        <v>4</v>
-      </c>
-      <c r="D16" s="4">
-        <v>1</v>
-      </c>
-      <c r="E16" s="7"/>
-      <c r="G16" s="12" t="s">
+      <c r="C18" s="4">
+        <v>4</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="7"/>
+      <c r="H18" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="H16" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
+      <c r="I18" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="4">
-        <v>4</v>
-      </c>
-      <c r="D17" s="4">
-        <v>1</v>
-      </c>
-      <c r="E17" s="7"/>
-      <c r="G17" s="12" t="s">
+      <c r="C19" s="4">
+        <v>4</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="7"/>
+      <c r="H19" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="H17" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
+      <c r="I19" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="4">
-        <v>4</v>
-      </c>
-      <c r="D18" s="4">
-        <v>1</v>
-      </c>
-      <c r="E18" s="7"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+      <c r="C20" s="4">
+        <v>4</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="4">
-        <v>4</v>
-      </c>
-      <c r="D19" s="4">
-        <v>1</v>
-      </c>
-      <c r="E19" s="7"/>
-      <c r="G19" s="9" t="s">
+      <c r="C21" s="4">
+        <v>4</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="7"/>
+      <c r="H21" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="H19" s="9"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+      <c r="I21" s="28"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="4">
-        <v>4</v>
-      </c>
-      <c r="D20" s="4">
-        <v>2</v>
-      </c>
-      <c r="E20" s="7"/>
-      <c r="G20" s="11" t="s">
+      <c r="C22" s="4">
+        <v>4</v>
+      </c>
+      <c r="D22" s="4">
+        <v>2</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="7"/>
+      <c r="H22" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="I22" s="10" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="4">
-        <v>4</v>
-      </c>
-      <c r="D21" s="4">
-        <v>2</v>
-      </c>
-      <c r="E21" s="7"/>
-      <c r="G21" s="12" t="s">
+      <c r="C23" s="4">
+        <v>4</v>
+      </c>
+      <c r="D23" s="4">
+        <v>2</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="7"/>
+      <c r="H23" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="H21" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
+      <c r="I23" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B24" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="4">
-        <v>4</v>
-      </c>
-      <c r="D22" s="4">
-        <v>2</v>
-      </c>
-      <c r="E22" s="7"/>
-      <c r="G22" s="12" t="s">
+      <c r="C24" s="4">
+        <v>4</v>
+      </c>
+      <c r="D24" s="4">
+        <v>2</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="7"/>
+      <c r="H24" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="H22" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="27" t="s">
+      <c r="I24" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="4">
-        <v>4</v>
-      </c>
-      <c r="D23" s="4">
-        <v>2</v>
-      </c>
-      <c r="E23" s="7"/>
-      <c r="G23" s="12" t="s">
+      <c r="C25" s="4">
+        <v>4</v>
+      </c>
+      <c r="D25" s="4">
+        <v>2</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="7"/>
+      <c r="H25" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="H23" s="12">
+      <c r="I25" s="11">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
         <v>5</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B26" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="23"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="27"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="4">
-        <v>4</v>
-      </c>
-      <c r="D25" s="4">
-        <v>2</v>
-      </c>
-      <c r="E25" s="7"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
+      <c r="C27" s="4">
+        <v>4</v>
+      </c>
+      <c r="D27" s="4">
+        <v>2</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="4">
-        <v>4</v>
-      </c>
-      <c r="D26" s="4">
-        <v>2</v>
-      </c>
-      <c r="E26" s="7"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="27" t="s">
+      <c r="C28" s="4">
+        <v>4</v>
+      </c>
+      <c r="D28" s="4">
+        <v>2</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="4">
-        <v>4</v>
-      </c>
-      <c r="D27" s="4">
-        <v>2</v>
-      </c>
-      <c r="E27" s="7"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
+      <c r="C29" s="4">
+        <v>4</v>
+      </c>
+      <c r="D29" s="4">
+        <v>2</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="9">
         <v>6</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B30" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="23"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="27" t="s">
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="27"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B31" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="4">
-        <v>4</v>
-      </c>
-      <c r="D29" s="4">
-        <v>2</v>
-      </c>
-      <c r="E29" s="7"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="27" t="s">
+      <c r="C31" s="4">
+        <v>4</v>
+      </c>
+      <c r="D31" s="4">
+        <v>2</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B32" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="4">
-        <v>4</v>
-      </c>
-      <c r="D30" s="4">
-        <v>2</v>
-      </c>
-      <c r="E30" s="7"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="27" t="s">
+      <c r="C32" s="4">
+        <v>4</v>
+      </c>
+      <c r="D32" s="4">
+        <v>2</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B33" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="4">
-        <v>4</v>
-      </c>
-      <c r="D31" s="4">
-        <v>2</v>
-      </c>
-      <c r="E31" s="7"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="27" t="s">
+      <c r="C33" s="4">
+        <v>4</v>
+      </c>
+      <c r="D33" s="4">
+        <v>2</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B34" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="4">
-        <v>4</v>
-      </c>
-      <c r="D32" s="4">
-        <v>2</v>
-      </c>
-      <c r="E32" s="7"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="27" t="s">
+      <c r="C34" s="4">
+        <v>4</v>
+      </c>
+      <c r="D34" s="4">
+        <v>2</v>
+      </c>
+      <c r="E34" s="4"/>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="4">
-        <v>4</v>
-      </c>
-      <c r="D33" s="4">
-        <v>2</v>
-      </c>
-      <c r="E33" s="7"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="27" t="s">
+      <c r="C35" s="4">
+        <v>4</v>
+      </c>
+      <c r="D35" s="4">
+        <v>2</v>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="4">
-        <v>4</v>
-      </c>
-      <c r="D34" s="4">
-        <v>2</v>
-      </c>
-      <c r="E34" s="7"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="27" t="s">
+      <c r="C36" s="4">
+        <v>4</v>
+      </c>
+      <c r="D36" s="4">
+        <v>2</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="4">
-        <v>4</v>
-      </c>
-      <c r="D35" s="4">
-        <v>2</v>
-      </c>
-      <c r="E35" s="7"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="27" t="s">
+      <c r="C37" s="4">
+        <v>4</v>
+      </c>
+      <c r="D37" s="4">
+        <v>2</v>
+      </c>
+      <c r="E37" s="4"/>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C36" s="4">
-        <v>4</v>
-      </c>
-      <c r="D36" s="4">
-        <v>2</v>
-      </c>
-      <c r="E36" s="7"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="27" t="s">
+      <c r="C38" s="4">
+        <v>4</v>
+      </c>
+      <c r="D38" s="4">
+        <v>2</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="4">
-        <v>4</v>
-      </c>
-      <c r="D37" s="4">
-        <v>2</v>
-      </c>
-      <c r="E37" s="7"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="27" t="s">
+      <c r="C39" s="4">
+        <v>4</v>
+      </c>
+      <c r="D39" s="4">
+        <v>2</v>
+      </c>
+      <c r="E39" s="4"/>
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C38" s="4">
-        <v>4</v>
-      </c>
-      <c r="D38" s="4">
-        <v>2</v>
-      </c>
-      <c r="E38" s="7"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="27" t="s">
+      <c r="C40" s="4">
+        <v>4</v>
+      </c>
+      <c r="D40" s="4">
+        <v>2</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B41" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C39" s="4">
-        <v>4</v>
-      </c>
-      <c r="D39" s="4">
-        <v>2</v>
-      </c>
-      <c r="E39" s="7"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="27" t="s">
+      <c r="C41" s="4">
+        <v>4</v>
+      </c>
+      <c r="D41" s="4">
+        <v>2</v>
+      </c>
+      <c r="E41" s="4"/>
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C40" s="4">
-        <v>4</v>
-      </c>
-      <c r="D40" s="4">
-        <v>2</v>
-      </c>
-      <c r="E40" s="7"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="27" t="s">
+      <c r="C42" s="4">
+        <v>4</v>
+      </c>
+      <c r="D42" s="4">
+        <v>2</v>
+      </c>
+      <c r="E42" s="4"/>
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B43" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="C41" s="4">
-        <v>4</v>
-      </c>
-      <c r="D41" s="4">
-        <v>3</v>
-      </c>
-      <c r="E41" s="7"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C42" s="4">
-        <v>4</v>
-      </c>
-      <c r="D42" s="4">
-        <v>3</v>
-      </c>
-      <c r="E42" s="7"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="C43" s="4">
         <v>4</v>
@@ -1675,25 +1783,31 @@
       <c r="D43" s="4">
         <v>3</v>
       </c>
-      <c r="E43" s="7"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="10">
-        <v>7</v>
-      </c>
-      <c r="B44" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="23"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="27" t="s">
-        <v>78</v>
+      <c r="E43" s="4"/>
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C44" s="4">
+        <v>4</v>
+      </c>
+      <c r="D44" s="4">
+        <v>3</v>
+      </c>
+      <c r="E44" s="4"/>
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="23" t="s">
+        <v>76</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C45" s="4">
         <v>4</v>
@@ -1701,29 +1815,27 @@
       <c r="D45" s="4">
         <v>3</v>
       </c>
-      <c r="E45" s="7"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C46" s="4">
-        <v>4</v>
-      </c>
-      <c r="D46" s="4">
-        <v>3</v>
-      </c>
-      <c r="E46" s="7"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="27" t="s">
-        <v>87</v>
+      <c r="E45" s="4"/>
+      <c r="F45" s="7"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="9">
+        <v>7</v>
+      </c>
+      <c r="B46" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="27"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="23" t="s">
+        <v>78</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C47" s="4">
         <v>4</v>
@@ -1731,14 +1843,15 @@
       <c r="D47" s="4">
         <v>3</v>
       </c>
-      <c r="E47" s="7"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="27" t="s">
-        <v>88</v>
+      <c r="E47" s="4"/>
+      <c r="F47" s="7"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="23" t="s">
+        <v>86</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C48" s="4">
         <v>4</v>
@@ -1746,14 +1859,15 @@
       <c r="D48" s="4">
         <v>3</v>
       </c>
-      <c r="E48" s="7"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="27" t="s">
-        <v>89</v>
+      <c r="E48" s="4"/>
+      <c r="F48" s="7"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="23" t="s">
+        <v>87</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C49" s="4">
         <v>4</v>
@@ -1761,14 +1875,15 @@
       <c r="D49" s="4">
         <v>3</v>
       </c>
-      <c r="E49" s="7"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="27" t="s">
-        <v>90</v>
+      <c r="E49" s="4"/>
+      <c r="F49" s="7"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="23" t="s">
+        <v>88</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C50" s="4">
         <v>4</v>
@@ -1776,14 +1891,15 @@
       <c r="D50" s="4">
         <v>3</v>
       </c>
-      <c r="E50" s="7"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="27" t="s">
-        <v>91</v>
+      <c r="E50" s="4"/>
+      <c r="F50" s="7"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="23" t="s">
+        <v>89</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C51" s="4">
         <v>4</v>
@@ -1791,25 +1907,31 @@
       <c r="D51" s="4">
         <v>3</v>
       </c>
-      <c r="E51" s="7"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="10">
-        <v>8</v>
-      </c>
-      <c r="B52" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="C52" s="22"/>
-      <c r="D52" s="22"/>
-      <c r="E52" s="23"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="27" t="s">
-        <v>93</v>
+      <c r="E51" s="4"/>
+      <c r="F51" s="7"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C52" s="4">
+        <v>4</v>
+      </c>
+      <c r="D52" s="4">
+        <v>3</v>
+      </c>
+      <c r="E52" s="4"/>
+      <c r="F52" s="7"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="23" t="s">
+        <v>91</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C53" s="4">
         <v>4</v>
@@ -1817,29 +1939,27 @@
       <c r="D53" s="4">
         <v>3</v>
       </c>
-      <c r="E53" s="7"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C54" s="4">
-        <v>4</v>
-      </c>
-      <c r="D54" s="4">
-        <v>3</v>
-      </c>
-      <c r="E54" s="7"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="27" t="s">
-        <v>99</v>
+      <c r="E53" s="4"/>
+      <c r="F53" s="7"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="9">
+        <v>8</v>
+      </c>
+      <c r="B54" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="27"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="23" t="s">
+        <v>93</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C55" s="4">
         <v>4</v>
@@ -1847,34 +1967,69 @@
       <c r="D55" s="4">
         <v>3</v>
       </c>
-      <c r="E55" s="7"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="28" t="s">
+      <c r="E55" s="4"/>
+      <c r="F55" s="7"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C56" s="4">
+        <v>4</v>
+      </c>
+      <c r="D56" s="4">
+        <v>3</v>
+      </c>
+      <c r="E56" s="4"/>
+      <c r="F56" s="7"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C57" s="4">
+        <v>4</v>
+      </c>
+      <c r="D57" s="4">
+        <v>3</v>
+      </c>
+      <c r="E57" s="4"/>
+      <c r="F57" s="7"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B58" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C56" s="6">
-        <v>4</v>
-      </c>
-      <c r="D56" s="6">
+      <c r="C58" s="6">
+        <v>4</v>
+      </c>
+      <c r="D58" s="6">
         <v>3</v>
       </c>
-      <c r="E56" s="8"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="B52:E52"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="B14:E14"/>
+  <mergeCells count="10">
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Gean Pereira] - Refatoração de documentos
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso e Incrementos.xlsx
+++ b/Priorização de Casos de Uso e Incrementos.xlsx
@@ -580,9 +580,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -612,6 +609,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -621,19 +633,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -943,7 +943,7 @@
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D13" sqref="A3:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,85 +957,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="G1" s="9" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="G1" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="9"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="25">
+      <c r="A3" s="21">
         <v>1</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="19">
-        <v>4</v>
-      </c>
-      <c r="D3" s="19">
+      <c r="B3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="18">
+        <v>4</v>
+      </c>
+      <c r="D3" s="18">
         <v>1</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="G3" s="12">
+      <c r="E3" s="19"/>
+      <c r="G3" s="11">
         <v>1</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="13">
         <v>42019</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="26">
-        <v>2</v>
-      </c>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="22">
+        <v>2</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="16">
-        <v>4</v>
-      </c>
-      <c r="D4" s="16">
+      <c r="C4" s="15">
+        <v>4</v>
+      </c>
+      <c r="D4" s="15">
         <v>1</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="G4" s="12">
-        <v>2</v>
-      </c>
-      <c r="H4" s="14">
+      <c r="E4" s="16"/>
+      <c r="G4" s="11">
+        <v>2</v>
+      </c>
+      <c r="H4" s="13">
         <v>42026</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="27">
+      <c r="A5" s="23">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1048,15 +1048,15 @@
         <v>1</v>
       </c>
       <c r="E5" s="7"/>
-      <c r="G5" s="12">
+      <c r="G5" s="11">
         <v>3</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="13">
         <v>42033</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="23" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1073,7 +1073,7 @@
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1088,7 +1088,7 @@
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="23" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1103,7 +1103,7 @@
       <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="23" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1118,7 +1118,7 @@
       <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="23" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1133,7 +1133,7 @@
       <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="23" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1148,7 +1148,7 @@
       <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="23" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1161,13 +1161,13 @@
         <v>1</v>
       </c>
       <c r="E12" s="7"/>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="H12" s="9"/>
+      <c r="H12" s="28"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="23" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1180,32 +1180,32 @@
         <v>1</v>
       </c>
       <c r="E13" s="7"/>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="12" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
-        <v>4</v>
-      </c>
-      <c r="B14" s="21" t="s">
+      <c r="A14" s="9">
+        <v>4</v>
+      </c>
+      <c r="B14" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="23"/>
-      <c r="G14" s="12" t="s">
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="27"/>
+      <c r="G14" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="11">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="23" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1215,18 +1215,18 @@
         <v>4</v>
       </c>
       <c r="D15" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" s="7"/>
-      <c r="G15" s="12" t="s">
+      <c r="G15" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="11">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="23" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1236,18 +1236,18 @@
         <v>4</v>
       </c>
       <c r="D16" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" s="7"/>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="11">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="23" t="s">
         <v>25</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1257,18 +1257,18 @@
         <v>4</v>
       </c>
       <c r="D17" s="4">
+        <v>2</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="G17" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="H17" s="11">
         <v>1</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="G17" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="H17" s="12">
-        <v>1</v>
-      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="23" t="s">
         <v>27</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -1278,12 +1278,12 @@
         <v>4</v>
       </c>
       <c r="D18" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="23" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1293,16 +1293,16 @@
         <v>4</v>
       </c>
       <c r="D19" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" s="7"/>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="H19" s="9"/>
+      <c r="H19" s="28"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="23" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -1315,15 +1315,15 @@
         <v>2</v>
       </c>
       <c r="E20" s="7"/>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="10" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="23" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -1336,15 +1336,15 @@
         <v>2</v>
       </c>
       <c r="E21" s="7"/>
-      <c r="G21" s="12" t="s">
+      <c r="G21" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="H21" s="12">
+      <c r="H21" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="23" t="s">
         <v>35</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1357,15 +1357,15 @@
         <v>2</v>
       </c>
       <c r="E22" s="7"/>
-      <c r="G22" s="12" t="s">
+      <c r="G22" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="H22" s="12">
+      <c r="H22" s="11">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="23" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1378,26 +1378,26 @@
         <v>2</v>
       </c>
       <c r="E23" s="7"/>
-      <c r="G23" s="12" t="s">
+      <c r="G23" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="11">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
+      <c r="A24" s="9">
         <v>5</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="23"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="27"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="23" t="s">
         <v>40</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -1412,7 +1412,7 @@
       <c r="E25" s="7"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="23" t="s">
         <v>42</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -1427,7 +1427,7 @@
       <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="23" t="s">
         <v>44</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -1442,18 +1442,18 @@
       <c r="E27" s="7"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
+      <c r="A28" s="9">
         <v>6</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="23"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="27"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="23" t="s">
         <v>47</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -1468,7 +1468,7 @@
       <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="23" t="s">
         <v>48</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -1483,7 +1483,7 @@
       <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="23" t="s">
         <v>49</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -1498,7 +1498,7 @@
       <c r="E31" s="7"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="23" t="s">
         <v>50</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -1513,7 +1513,7 @@
       <c r="E32" s="7"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="23" t="s">
         <v>51</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -1528,7 +1528,7 @@
       <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="27" t="s">
+      <c r="A34" s="23" t="s">
         <v>52</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -1543,7 +1543,7 @@
       <c r="E34" s="7"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="23" t="s">
         <v>53</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -1558,7 +1558,7 @@
       <c r="E35" s="7"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="27" t="s">
+      <c r="A36" s="23" t="s">
         <v>54</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -1573,7 +1573,7 @@
       <c r="E36" s="7"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="27" t="s">
+      <c r="A37" s="23" t="s">
         <v>55</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -1588,7 +1588,7 @@
       <c r="E37" s="7"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="27" t="s">
+      <c r="A38" s="23" t="s">
         <v>56</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -1603,7 +1603,7 @@
       <c r="E38" s="7"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="27" t="s">
+      <c r="A39" s="23" t="s">
         <v>57</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -1618,7 +1618,7 @@
       <c r="E39" s="7"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="27" t="s">
+      <c r="A40" s="23" t="s">
         <v>58</v>
       </c>
       <c r="B40" s="3" t="s">
@@ -1633,7 +1633,7 @@
       <c r="E40" s="7"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="27" t="s">
+      <c r="A41" s="23" t="s">
         <v>59</v>
       </c>
       <c r="B41" s="3" t="s">
@@ -1648,7 +1648,7 @@
       <c r="E41" s="7"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="27" t="s">
+      <c r="A42" s="23" t="s">
         <v>75</v>
       </c>
       <c r="B42" s="3" t="s">
@@ -1663,7 +1663,7 @@
       <c r="E42" s="7"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="27" t="s">
+      <c r="A43" s="23" t="s">
         <v>76</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -1678,18 +1678,18 @@
       <c r="E43" s="7"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="10">
+      <c r="A44" s="9">
         <v>7</v>
       </c>
-      <c r="B44" s="21" t="s">
+      <c r="B44" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="23"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="27"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="27" t="s">
+      <c r="A45" s="23" t="s">
         <v>78</v>
       </c>
       <c r="B45" s="3" t="s">
@@ -1704,7 +1704,7 @@
       <c r="E45" s="7"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="27" t="s">
+      <c r="A46" s="23" t="s">
         <v>86</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -1719,7 +1719,7 @@
       <c r="E46" s="7"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="27" t="s">
+      <c r="A47" s="23" t="s">
         <v>87</v>
       </c>
       <c r="B47" s="3" t="s">
@@ -1734,7 +1734,7 @@
       <c r="E47" s="7"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="27" t="s">
+      <c r="A48" s="23" t="s">
         <v>88</v>
       </c>
       <c r="B48" s="3" t="s">
@@ -1749,7 +1749,7 @@
       <c r="E48" s="7"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="27" t="s">
+      <c r="A49" s="23" t="s">
         <v>89</v>
       </c>
       <c r="B49" s="3" t="s">
@@ -1764,7 +1764,7 @@
       <c r="E49" s="7"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="27" t="s">
+      <c r="A50" s="23" t="s">
         <v>90</v>
       </c>
       <c r="B50" s="3" t="s">
@@ -1779,7 +1779,7 @@
       <c r="E50" s="7"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="27" t="s">
+      <c r="A51" s="23" t="s">
         <v>91</v>
       </c>
       <c r="B51" s="3" t="s">
@@ -1794,18 +1794,18 @@
       <c r="E51" s="7"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="10">
+      <c r="A52" s="9">
         <v>8</v>
       </c>
-      <c r="B52" s="21" t="s">
+      <c r="B52" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="C52" s="22"/>
-      <c r="D52" s="22"/>
-      <c r="E52" s="23"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="27"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="27" t="s">
+      <c r="A53" s="23" t="s">
         <v>93</v>
       </c>
       <c r="B53" s="3" t="s">
@@ -1820,7 +1820,7 @@
       <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="27" t="s">
+      <c r="A54" s="23" t="s">
         <v>98</v>
       </c>
       <c r="B54" s="3" t="s">
@@ -1835,7 +1835,7 @@
       <c r="E54" s="7"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="27" t="s">
+      <c r="A55" s="23" t="s">
         <v>99</v>
       </c>
       <c r="B55" s="3" t="s">
@@ -1850,7 +1850,7 @@
       <c r="E55" s="7"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="28" t="s">
+      <c r="A56" s="24" t="s">
         <v>100</v>
       </c>
       <c r="B56" s="5" t="s">
@@ -1866,15 +1866,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="B14:E14"/>
     <mergeCell ref="B24:E24"/>
     <mergeCell ref="B28:E28"/>
     <mergeCell ref="B44:E44"/>
     <mergeCell ref="B52:E52"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="B14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>